<commit_message>
Updated yaml file to new naming conventions, versioning, and amazon endpoints. Updated xlsx file with amazon endpoints
</commit_message>
<xml_diff>
--- a/veranda_API_endpoints.xlsx
+++ b/veranda_API_endpoints.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patrick\Desktop\veranda\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patrick\Desktop\veranda\veranda-api-documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95432481-1CB4-4615-BDB6-4C5A2548D11B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99E94DB3-781E-460E-8DBC-3A4C56CB8D08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0344EC85-21F1-455F-B794-86C4A379A39B}"/>
+    <workbookView xWindow="12045" yWindow="810" windowWidth="21630" windowHeight="13665" xr2:uid="{0344EC85-21F1-455F-B794-86C4A379A39B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="56">
   <si>
     <t>Admin</t>
   </si>
@@ -48,39 +48,18 @@
     <t>Endpoint name</t>
   </si>
   <si>
-    <t>/admin/lock</t>
-  </si>
-  <si>
     <t>POST</t>
   </si>
   <si>
-    <t>lock.createLock</t>
-  </si>
-  <si>
     <t>Path</t>
   </si>
   <si>
-    <t>/admin/lock/{id}</t>
-  </si>
-  <si>
     <t>GET</t>
   </si>
   <si>
-    <t>lock.getLock</t>
-  </si>
-  <si>
     <t>Delete</t>
   </si>
   <si>
-    <t>lock.deleteLock</t>
-  </si>
-  <si>
-    <t>/admin/lock/{id}/version</t>
-  </si>
-  <si>
-    <t>versioning.getLockVersion</t>
-  </si>
-  <si>
     <t>Cognito</t>
   </si>
   <si>
@@ -99,91 +78,130 @@
     <t>LoRa</t>
   </si>
   <si>
-    <t>/lora-uplink</t>
-  </si>
-  <si>
-    <t>lock_telemetry.loraUplink</t>
-  </si>
-  <si>
     <t>Client</t>
   </si>
   <si>
     <t>n/a</t>
   </si>
   <si>
-    <t>/profile</t>
-  </si>
-  <si>
-    <t>app_users.getProfile</t>
-  </si>
-  <si>
-    <t>/locks/owned</t>
-  </si>
-  <si>
-    <t>/locks/shared</t>
-  </si>
-  <si>
-    <t>lock_roles.sharedLocks</t>
-  </si>
-  <si>
-    <t>lock_roles.ownedLocks</t>
-  </si>
-  <si>
-    <t>/locks/{id}</t>
-  </si>
-  <si>
-    <t>lock_roles.getLock</t>
-  </si>
-  <si>
     <t>PUT</t>
   </si>
   <si>
-    <t>lock_roles.changeLockName</t>
-  </si>
-  <si>
-    <t>/locks/register/{reg_id}</t>
-  </si>
-  <si>
-    <t>lock_roles.registerLock</t>
-  </si>
-  <si>
-    <t>lock_roles.deregisterLock</t>
-  </si>
-  <si>
-    <t>/locks/{id}/shared-users</t>
-  </si>
-  <si>
-    <t>lock_roles.addSharedUser</t>
-  </si>
-  <si>
-    <t>lock_roles.removeSharedUser</t>
-  </si>
-  <si>
-    <t>lock_roles.getSharedUsers</t>
-  </si>
-  <si>
-    <t>lock_roles.deleteSharedLock</t>
-  </si>
-  <si>
-    <t>/locks/{id}/telemetry</t>
-  </si>
-  <si>
-    <t>lock_telemetry.getLockTelemetry</t>
-  </si>
-  <si>
-    <t>lock_usage_record.getLockLogs</t>
-  </si>
-  <si>
-    <t>/locks/{id}/unlock</t>
-  </si>
-  <si>
-    <t>lock_usage_record.unlockLock</t>
-  </si>
-  <si>
-    <t>/locks/{id}/connectivity-logs</t>
-  </si>
-  <si>
-    <t>/locks/shared/{id}</t>
+    <t>Scraping</t>
+  </si>
+  <si>
+    <t>/v1/admin/lock</t>
+  </si>
+  <si>
+    <t>/v1/admin/lock/{id}</t>
+  </si>
+  <si>
+    <t>/v1/admin/lock/{id}/version</t>
+  </si>
+  <si>
+    <t>/v1/lora-uplink</t>
+  </si>
+  <si>
+    <t>/v1/profile</t>
+  </si>
+  <si>
+    <t>/v1/locks/owned</t>
+  </si>
+  <si>
+    <t>/v1/locks/shared</t>
+  </si>
+  <si>
+    <t>/v1/locks/shared/{id}</t>
+  </si>
+  <si>
+    <t>/v1/locks/{id}</t>
+  </si>
+  <si>
+    <t>/v1/locks/register/{reg_id}</t>
+  </si>
+  <si>
+    <t>/v1/locks/{id}/shared-users</t>
+  </si>
+  <si>
+    <t>/v1/locks/{id}/telemetry</t>
+  </si>
+  <si>
+    <t>/v1/locks/{id}/connectivity-logs</t>
+  </si>
+  <si>
+    <t>/v1/locks/{id}/unlock</t>
+  </si>
+  <si>
+    <t>/v1/orders/amazon</t>
+  </si>
+  <si>
+    <t>amazon_scrape.getAmazonOrders_v1</t>
+  </si>
+  <si>
+    <t>lock.createLock_v1</t>
+  </si>
+  <si>
+    <t>lock.getLock_v1</t>
+  </si>
+  <si>
+    <t>lock.deleteLock_v1</t>
+  </si>
+  <si>
+    <t>versioning.getLockVersion_v1</t>
+  </si>
+  <si>
+    <t>lock_telemetry.loraUplink_v1</t>
+  </si>
+  <si>
+    <t>lock_roles.ownedLocks_v1</t>
+  </si>
+  <si>
+    <t>app_users.getProfile_v1</t>
+  </si>
+  <si>
+    <t>lock_roles.sharedLocks_v1</t>
+  </si>
+  <si>
+    <t>lock_roles.deleteSharedLock_v1</t>
+  </si>
+  <si>
+    <t>lock_roles.getLock_v1</t>
+  </si>
+  <si>
+    <t>lock_roles.changeLockName_v1</t>
+  </si>
+  <si>
+    <t>lock_roles.registerLock_v1</t>
+  </si>
+  <si>
+    <t>lock_roles.deregisterLock_v1</t>
+  </si>
+  <si>
+    <t>lock_roles.addSharedUser_v1</t>
+  </si>
+  <si>
+    <t>lock_roles.removeSharedUser_v1</t>
+  </si>
+  <si>
+    <t>lock_roles.getSharedUsers_v1</t>
+  </si>
+  <si>
+    <t>lock_telemetry.getLockTelemetry_v1</t>
+  </si>
+  <si>
+    <t>lock_usage_record.getLockLogs_v1</t>
+  </si>
+  <si>
+    <t>lock_usage_record.unlockLock_v1</t>
+  </si>
+  <si>
+    <t>store_login.storeAmazonLogin_v1</t>
+  </si>
+  <si>
+    <t>store_login.removeAmazonLogin_v1</t>
+  </si>
+  <si>
+    <t>store_login.updateAmazonLogin_v1</t>
   </si>
 </sst>
 </file>
@@ -677,10 +695,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8796450E-0344-4247-9B58-5FFDD26827D3}">
-  <dimension ref="B2:M25"/>
+  <dimension ref="B2:M30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -701,7 +719,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>2</v>
@@ -710,13 +728,13 @@
         <v>3</v>
       </c>
       <c r="I3" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="J3" s="4" t="s">
         <v>1</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="L3" s="2" t="s">
         <v>2</v>
@@ -730,69 +748,69 @@
         <v>0</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="K4" s="11"/>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="7" t="s">
-        <v>5</v>
-      </c>
       <c r="E5" t="s">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="K5" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="L5" s="12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M5" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E6" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="L6" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="M6" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D7" s="8" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E7" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E8" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
@@ -800,56 +818,56 @@
         <v>21</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E10" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E12" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E13" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E14" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E15" t="s">
         <v>42</v>
@@ -857,100 +875,149 @@
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D17" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E18" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D19" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D21" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D22" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>29</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E23" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>30</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E24" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
         <v>31</v>
       </c>
-      <c r="D16" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E16" t="s">
+      <c r="D25" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E25" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D17" s="13" t="s">
+      <c r="D27" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E27" t="s">
         <v>33</v>
       </c>
-      <c r="E17" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C18" t="s">
-        <v>35</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E18" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D19" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E19" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C20" t="s">
-        <v>38</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E20" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="21" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D21" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E21" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="22" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D22" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E22" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="23" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C23" t="s">
-        <v>43</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E23" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="24" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C24" t="s">
-        <v>48</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E24" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="25" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C25" t="s">
-        <v>46</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E25" t="s">
-        <v>47</v>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>32</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E28" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>32</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E29" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>32</v>
+      </c>
+      <c r="D30" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E30" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Final push for last endpoint documentation
</commit_message>
<xml_diff>
--- a/veranda_API_endpoints.xlsx
+++ b/veranda_API_endpoints.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patrick\Desktop\veranda\veranda-api-documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99E94DB3-781E-460E-8DBC-3A4C56CB8D08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D8BBFBE-54BE-43E1-BE93-B25B9230C42E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12045" yWindow="810" windowWidth="21630" windowHeight="13665" xr2:uid="{0344EC85-21F1-455F-B794-86C4A379A39B}"/>
+    <workbookView xWindow="-23235" yWindow="345" windowWidth="21630" windowHeight="13665" xr2:uid="{0344EC85-21F1-455F-B794-86C4A379A39B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="58">
   <si>
     <t>Admin</t>
   </si>
@@ -202,6 +202,12 @@
   </si>
   <si>
     <t>store_login.updateAmazonLogin_v1</t>
+  </si>
+  <si>
+    <t>/v1/orders/amazon/creds</t>
+  </si>
+  <si>
+    <t>store_login.checkForAmazonCredentials_v1</t>
   </si>
 </sst>
 </file>
@@ -695,10 +701,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8796450E-0344-4247-9B58-5FFDD26827D3}">
-  <dimension ref="B2:M30"/>
+  <dimension ref="B2:M31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -989,34 +995,45 @@
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
-        <v>32</v>
-      </c>
-      <c r="D28" s="7" t="s">
-        <v>4</v>
+        <v>56</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>6</v>
       </c>
       <c r="E28" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
-        <v>32</v>
-      </c>
-      <c r="D29" s="8" t="s">
-        <v>7</v>
+        <v>56</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>4</v>
       </c>
       <c r="E29" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
-        <v>32</v>
-      </c>
-      <c r="D30" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E30" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>56</v>
+      </c>
+      <c r="D31" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E31" t="s">
         <v>55</v>
       </c>
     </row>

</xml_diff>